<commit_message>
Adding the 2 Bert model features and changeing pipeline to only take the union of top 100 of bm24 tf and pl2
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,45 @@
         <v>0.4328666394185419</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>(TerrierRetr(BM25) &gt;&gt; (TerrierRetr(Tf) ** TerrierRetr(PL2) ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score()) &gt;&gt; &lt;pyterrier.ltr.LTRTransformer object at 0x000001A33AE4CAD0&gt;)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2636832138379338</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.4328666394185419</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>(&lt;pyterrier._ops.SetUnion object at 0x000001949B4976F0&gt; &gt;&gt; &lt;pyterrier.terrier._text_loader.TerrierTextLoader object at 0x00000194A6A5FC50&gt; &gt;&gt; (&lt;pyterrier.terrier.retriever.TextScorer object at 0x000001949B4975C0&gt; ** &lt;pyterrier.terrier.retriever.TextScorer object at 0x000001949B496EA0&gt; ** &lt;pyterrier.terrier.retriever.TextScorer object at 0x0000019496D74A70&gt; ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score()) &gt;&gt; &lt;pyterrier.ltr.LTRTransformer object at 0x00000194A6A5F110&gt;)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.09141840205407331</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3209493560511296</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>(&lt;pyterrier._ops.SetUnion object at 0x0000019251400050&gt; &gt;&gt; &lt;pyterrier.terrier._text_loader.TerrierTextLoader object at 0x00000192514B97F0&gt; &gt;&gt; (&lt;pyterrier.terrier.retriever.TextScorer object at 0x00000192514B9550&gt; ** &lt;pyterrier.terrier.retriever.TextScorer object at 0x0000019251400190&gt; ** &lt;pyterrier.terrier.retriever.TextScorer object at 0x00000192514002D0&gt; ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score() ** pt.apply.doc_score()) &gt;&gt; &lt;pyterrier.ltr.LTRTransformer object at 0x00000192514B9A90&gt;)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.2743828363576117</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.4760306064989383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>